<commit_message>
Update simulation case 5 files
</commit_message>
<xml_diff>
--- a/SimulationStudyData/Model1/SimCase5_zsim_SimRun1.xlsx
+++ b/SimulationStudyData/Model1/SimCase5_zsim_SimRun1.xlsx
@@ -358,7 +358,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
@@ -373,32 +373,32 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -408,12 +408,12 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15">
@@ -423,7 +423,7 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17">
@@ -433,12 +433,12 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20">
@@ -453,7 +453,7 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23">
@@ -468,37 +468,37 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="32">
@@ -508,7 +508,7 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34">
@@ -518,17 +518,17 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="38">
@@ -538,7 +538,7 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40">
@@ -548,12 +548,12 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43">
@@ -583,17 +583,17 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="51">
@@ -603,32 +603,32 @@
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="58">
@@ -643,7 +643,7 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61">
@@ -653,7 +653,7 @@
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="63">
@@ -673,7 +673,7 @@
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="67">
@@ -683,52 +683,52 @@
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="78">
@@ -743,22 +743,22 @@
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="84">
@@ -773,17 +773,17 @@
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="89">
@@ -803,7 +803,7 @@
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93">
@@ -828,7 +828,7 @@
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="98">
@@ -843,7 +843,7 @@
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="101">
@@ -853,7 +853,7 @@
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="103">
@@ -868,17 +868,17 @@
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="108">
@@ -888,17 +888,17 @@
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112">
@@ -908,32 +908,32 @@
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="119">
@@ -948,37 +948,37 @@
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="128">
@@ -988,52 +988,52 @@
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="139">
@@ -1048,17 +1048,17 @@
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="144">
@@ -1073,12 +1073,12 @@
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="148">
@@ -1088,12 +1088,12 @@
     </row>
     <row r="149">
       <c r="A149" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="151">
@@ -1103,7 +1103,7 @@
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="153">
@@ -1113,7 +1113,7 @@
     </row>
     <row r="154">
       <c r="A154" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="155">
@@ -1123,7 +1123,7 @@
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="157">
@@ -1133,7 +1133,7 @@
     </row>
     <row r="158">
       <c r="A158" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="159">
@@ -1143,7 +1143,7 @@
     </row>
     <row r="160">
       <c r="A160" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="161">
@@ -1153,7 +1153,7 @@
     </row>
     <row r="162">
       <c r="A162" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="163">
@@ -1163,12 +1163,12 @@
     </row>
     <row r="164">
       <c r="A164" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="166">
@@ -1178,32 +1178,32 @@
     </row>
     <row r="167">
       <c r="A167" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="173">
@@ -1213,7 +1213,7 @@
     </row>
     <row r="174">
       <c r="A174" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="175">
@@ -1228,7 +1228,7 @@
     </row>
     <row r="177">
       <c r="A177" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="178">
@@ -1243,12 +1243,12 @@
     </row>
     <row r="180">
       <c r="A180" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="182">
@@ -1258,12 +1258,12 @@
     </row>
     <row r="183">
       <c r="A183" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="185">
@@ -1273,22 +1273,22 @@
     </row>
     <row r="186">
       <c r="A186" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="190">
@@ -1298,12 +1298,12 @@
     </row>
     <row r="191">
       <c r="A191" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="193">
@@ -1313,27 +1313,27 @@
     </row>
     <row r="194">
       <c r="A194" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="199">
@@ -1343,262 +1343,12 @@
     </row>
     <row r="200">
       <c r="A200" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="202">
-      <c r="A202" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="203">
-      <c r="A203" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="204">
-      <c r="A204" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="205">
-      <c r="A205" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="206">
-      <c r="A206" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="207">
-      <c r="A207" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="208">
-      <c r="A208" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="209">
-      <c r="A209" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="210">
-      <c r="A210" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="211">
-      <c r="A211" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="212">
-      <c r="A212" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="213">
-      <c r="A213" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="214">
-      <c r="A214" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="215">
-      <c r="A215" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="216">
-      <c r="A216" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="217">
-      <c r="A217" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="218">
-      <c r="A218" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="219">
-      <c r="A219" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="220">
-      <c r="A220" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="221">
-      <c r="A221" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="222">
-      <c r="A222" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="223">
-      <c r="A223" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="224">
-      <c r="A224" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="225">
-      <c r="A225" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="226">
-      <c r="A226" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="227">
-      <c r="A227" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="228">
-      <c r="A228" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="229">
-      <c r="A229" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="230">
-      <c r="A230" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="231">
-      <c r="A231" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="232">
-      <c r="A232" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="233">
-      <c r="A233" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="234">
-      <c r="A234" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="235">
-      <c r="A235" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="236">
-      <c r="A236" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="237">
-      <c r="A237" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="238">
-      <c r="A238" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="239">
-      <c r="A239" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="240">
-      <c r="A240" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="241">
-      <c r="A241" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="242">
-      <c r="A242" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="243">
-      <c r="A243" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="244">
-      <c r="A244" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="245">
-      <c r="A245" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="246">
-      <c r="A246" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="247">
-      <c r="A247" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="248">
-      <c r="A248" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="249">
-      <c r="A249" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="250">
-      <c r="A250" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="251">
-      <c r="A251" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>